<commit_message>
Initial commit - chatbot_amdec_gamme
</commit_message>
<xml_diff>
--- a/data/models/amdec_generated.xlsx
+++ b/data/models/amdec_generated.xlsx
@@ -549,7 +549,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Maintenance corrective + Contrôle ultrasons</t>
+          <t>Maintenance corrective + Soudure inox</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Maintenance corrective + Nettoyage chimique</t>
+          <t>Maintenance corrective + Analyse des dépôts</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Maintenance corrective + Modification des supports</t>
+          <t>Maintenance corrective + Surveillance vibratoire</t>
         </is>
       </c>
     </row>

</xml_diff>